<commit_message>
ejercicios de excel filtros avanzados
</commit_message>
<xml_diff>
--- a/m1/u1/ejercicios/20191106/Alquiler coches.xlsx
+++ b/m1/u1/ejercicios/20191106/Alquiler coches.xlsx
@@ -476,58 +476,58 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Euro" xfId="2"/>
@@ -968,7 +968,7 @@
   <dimension ref="B1:H24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+      <selection activeCell="D12" sqref="D12:D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -983,10 +983,10 @@
   <sheetData>
     <row r="1" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="21"/>
+      <c r="C2" s="25"/>
       <c r="E2" s="4" t="s">
         <v>0</v>
       </c>
@@ -1059,25 +1059,25 @@
       <c r="C7" s="11">
         <v>43784</v>
       </c>
-      <c r="E7" s="34">
+      <c r="E7" s="20">
         <f>IF(WEEKDAY(C7,2)&lt;6,2%,0)</f>
         <v>0.02</v>
       </c>
-      <c r="F7" s="36">
+      <c r="F7" s="22">
         <f>IF(C6&gt;4,5%,0)</f>
         <v>0</v>
       </c>
-      <c r="G7" s="36">
+      <c r="G7" s="22">
         <f>IF(C4&gt;=30,10%,0)</f>
         <v>0</v>
       </c>
-      <c r="H7" s="36">
+      <c r="H7" s="22">
         <f>IF(C5="Mujer",15%,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="E8" s="39"/>
+      <c r="E8" s="23"/>
     </row>
     <row r="10" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="11" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1087,34 +1087,34 @@
       <c r="E11" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="F11" s="32" t="s">
+      <c r="F11" s="38" t="s">
         <v>29</v>
       </c>
-      <c r="G11" s="33"/>
+      <c r="G11" s="39"/>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B12" s="22" t="s">
+      <c r="B12" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="23"/>
-      <c r="D12" s="37">
+      <c r="C12" s="27"/>
+      <c r="D12" s="30">
         <f ca="1">ABS(IF(SUM(E7:H7)&lt;&gt;0,(F3*F17)*SUM(E7:H7)-F3*F17,F3*F17))</f>
-        <v>352.8</v>
-      </c>
-      <c r="E12" s="26">
+        <v>313.60000000000002</v>
+      </c>
+      <c r="E12" s="32">
         <f>G3*G17*IF(AND(C4&lt;30,C6&lt;5),30%,IF(OR(C4&lt;30,C6&lt;5),10%,0))</f>
         <v>36</v>
       </c>
-      <c r="F12" s="28"/>
-      <c r="G12" s="29"/>
+      <c r="F12" s="34"/>
+      <c r="G12" s="35"/>
     </row>
     <row r="13" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="24"/>
-      <c r="C13" s="25"/>
-      <c r="D13" s="38"/>
-      <c r="E13" s="27"/>
-      <c r="F13" s="30"/>
-      <c r="G13" s="31"/>
+      <c r="B13" s="28"/>
+      <c r="C13" s="29"/>
+      <c r="D13" s="31"/>
+      <c r="E13" s="33"/>
+      <c r="F13" s="36"/>
+      <c r="G13" s="37"/>
     </row>
     <row r="15" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="16" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1144,9 +1144,9 @@
       <c r="D17" s="6">
         <v>0.25</v>
       </c>
-      <c r="F17" s="35">
+      <c r="F17" s="21">
         <f ca="1">C7-TODAY()</f>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G17" s="1">
         <v>400</v>
@@ -1184,7 +1184,7 @@
       <c r="D20" s="10">
         <v>0.22</v>
       </c>
-      <c r="G20" s="39"/>
+      <c r="G20" s="23"/>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G24">

</xml_diff>